<commit_message>
23/03/2017 Import from XLSX work
</commit_message>
<xml_diff>
--- a/import.xlsx
+++ b/import.xlsx
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,146 +487,11 @@
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-    </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="8"/>
+      <c r="C8" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>